<commit_message>
feat: plots boxplots for nutrients and mean errors
</commit_message>
<xml_diff>
--- a/sum_nutrients_per_app_and_dish.xlsx
+++ b/sum_nutrients_per_app_and_dish.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,15 +476,10 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>sum_fiber</t>
+          <t>sum_fats</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>sum_fats</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>sum_sodium</t>
         </is>
@@ -522,12 +517,9 @@
         <v>143.1999969482422</v>
       </c>
       <c r="I2" t="n">
-        <v>24</v>
+        <v>5.699999809265137</v>
       </c>
       <c r="J2" t="n">
-        <v>5.699999809265137</v>
-      </c>
-      <c r="K2" t="n">
         <v>997.4000244140625</v>
       </c>
     </row>
@@ -563,12 +555,9 @@
         <v>99.70000171661377</v>
       </c>
       <c r="I3" t="n">
-        <v>11.30000001192093</v>
+        <v>19</v>
       </c>
       <c r="J3" t="n">
-        <v>19</v>
-      </c>
-      <c r="K3" t="n">
         <v>1352.399963378906</v>
       </c>
     </row>
@@ -604,12 +593,9 @@
         <v>79</v>
       </c>
       <c r="I4" t="n">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="J4" t="n">
-        <v>47</v>
-      </c>
-      <c r="K4" t="n">
         <v>1459.400024414062</v>
       </c>
     </row>
@@ -644,12 +630,9 @@
         <v>43</v>
       </c>
       <c r="I5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" t="n">
         <v>880</v>
       </c>
     </row>
@@ -684,12 +667,9 @@
         <v>56</v>
       </c>
       <c r="I6" t="n">
-        <v>4</v>
+        <v>30.20000000298023</v>
       </c>
       <c r="J6" t="n">
-        <v>30.20000000298023</v>
-      </c>
-      <c r="K6" t="n">
         <v>698.8000030517578</v>
       </c>
     </row>
@@ -725,12 +705,9 @@
         <v>43</v>
       </c>
       <c r="I7" t="n">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="J7" t="n">
-        <v>54</v>
-      </c>
-      <c r="K7" t="n">
         <v>362.7999935150146</v>
       </c>
     </row>
@@ -766,12 +743,9 @@
         <v>105</v>
       </c>
       <c r="I8" t="n">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="J8" t="n">
-        <v>47</v>
-      </c>
-      <c r="K8" t="n">
         <v>1927.999938964844</v>
       </c>
     </row>
@@ -807,12 +781,9 @@
         <v>18</v>
       </c>
       <c r="I9" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J9" t="n">
-        <v>5</v>
-      </c>
-      <c r="K9" t="n">
         <v>39.59999847412109</v>
       </c>
     </row>
@@ -848,12 +819,9 @@
         <v>163.199999243021</v>
       </c>
       <c r="I10" t="n">
-        <v>10</v>
+        <v>72.00000038743019</v>
       </c>
       <c r="J10" t="n">
-        <v>72.00000038743019</v>
-      </c>
-      <c r="K10" t="n">
         <v>1749.500040054321</v>
       </c>
     </row>
@@ -889,12 +857,9 @@
         <v>49</v>
       </c>
       <c r="I11" t="n">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="J11" t="n">
-        <v>27</v>
-      </c>
-      <c r="K11" t="n">
         <v>669.4999694824219</v>
       </c>
     </row>
@@ -930,12 +895,9 @@
         <v>60.90000000596046</v>
       </c>
       <c r="I12" t="n">
-        <v>5.5</v>
+        <v>72.30000019073486</v>
       </c>
       <c r="J12" t="n">
-        <v>72.30000019073486</v>
-      </c>
-      <c r="K12" t="n">
         <v>534.9999847412109</v>
       </c>
     </row>
@@ -971,12 +933,9 @@
         <v>145</v>
       </c>
       <c r="I13" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J13" t="n">
-        <v>18</v>
-      </c>
-      <c r="K13" t="n">
         <v>306.2000064849854</v>
       </c>
     </row>
@@ -1012,12 +971,9 @@
         <v>69</v>
       </c>
       <c r="I14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J14" t="n">
-        <v>10</v>
-      </c>
-      <c r="K14" t="n">
         <v>289.5999984741211</v>
       </c>
     </row>
@@ -1053,12 +1009,9 @@
         <v>80</v>
       </c>
       <c r="I15" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="J15" t="n">
-        <v>27</v>
-      </c>
-      <c r="K15" t="n">
         <v>2056.399993896484</v>
       </c>
     </row>
@@ -1094,12 +1047,9 @@
         <v>116</v>
       </c>
       <c r="I16" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J16" t="n">
-        <v>22</v>
-      </c>
-      <c r="K16" t="n">
         <v>1970.49995136261</v>
       </c>
     </row>
@@ -1135,12 +1085,9 @@
         <v>76</v>
       </c>
       <c r="I17" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="J17" t="n">
-        <v>18</v>
-      </c>
-      <c r="K17" t="n">
         <v>637.7000122070312</v>
       </c>
     </row>
@@ -1176,12 +1123,9 @@
         <v>108</v>
       </c>
       <c r="I18" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="J18" t="n">
-        <v>42</v>
-      </c>
-      <c r="K18" t="n">
         <v>1598.400024414062</v>
       </c>
     </row>
@@ -1217,12 +1161,9 @@
         <v>73.89999961853027</v>
       </c>
       <c r="I19" t="n">
-        <v>12.09999990463257</v>
+        <v>9.399999633431435</v>
       </c>
       <c r="J19" t="n">
-        <v>9.399999633431435</v>
-      </c>
-      <c r="K19" t="n">
         <v>397.8999910354614</v>
       </c>
     </row>
@@ -1258,12 +1199,9 @@
         <v>183</v>
       </c>
       <c r="I20" t="n">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="J20" t="n">
-        <v>59</v>
-      </c>
-      <c r="K20" t="n">
         <v>1199.100006103516</v>
       </c>
     </row>
@@ -1299,12 +1237,9 @@
         <v>75.5</v>
       </c>
       <c r="I21" t="n">
-        <v>2.799999952316284</v>
+        <v>29</v>
       </c>
       <c r="J21" t="n">
-        <v>29</v>
-      </c>
-      <c r="K21" t="n">
         <v>1765.899948120117</v>
       </c>
     </row>
@@ -1340,12 +1275,9 @@
         <v>65.49999904632568</v>
       </c>
       <c r="I22" t="n">
-        <v>7.200000047683716</v>
+        <v>13.0000001937151</v>
       </c>
       <c r="J22" t="n">
-        <v>13.0000001937151</v>
-      </c>
-      <c r="K22" t="n">
         <v>442.8999910354614</v>
       </c>
     </row>
@@ -1381,12 +1313,9 @@
         <v>62</v>
       </c>
       <c r="I23" t="n">
-        <v>8.899999618530273</v>
+        <v>13.80000019073486</v>
       </c>
       <c r="J23" t="n">
-        <v>13.80000019073486</v>
-      </c>
-      <c r="K23" t="n">
         <v>1198</v>
       </c>
     </row>
@@ -1422,12 +1351,9 @@
         <v>73.79999923706055</v>
       </c>
       <c r="I24" t="n">
-        <v>10.09999990463257</v>
+        <v>25.80000077188015</v>
       </c>
       <c r="J24" t="n">
-        <v>25.80000077188015</v>
-      </c>
-      <c r="K24" t="n">
         <v>1840</v>
       </c>
     </row>
@@ -1463,12 +1389,9 @@
         <v>94.30000305175781</v>
       </c>
       <c r="I25" t="n">
-        <v>5.400000095367432</v>
+        <v>59.30000114440918</v>
       </c>
       <c r="J25" t="n">
-        <v>59.30000114440918</v>
-      </c>
-      <c r="K25" t="n">
         <v>839</v>
       </c>
     </row>
@@ -1503,12 +1426,9 @@
         <v>17.60000038146973</v>
       </c>
       <c r="I26" t="n">
-        <v>0.800000011920929</v>
+        <v>27</v>
       </c>
       <c r="J26" t="n">
-        <v>27</v>
-      </c>
-      <c r="K26" t="n">
         <v>1924</v>
       </c>
     </row>
@@ -1543,12 +1463,9 @@
         <v>62.40000152587891</v>
       </c>
       <c r="I27" t="n">
-        <v>9.299999952316284</v>
+        <v>14.79999983310699</v>
       </c>
       <c r="J27" t="n">
-        <v>14.79999983310699</v>
-      </c>
-      <c r="K27" t="n">
         <v>1822</v>
       </c>
     </row>
@@ -1584,12 +1501,9 @@
         <v>32.80000019073486</v>
       </c>
       <c r="I28" t="n">
-        <v>5.99999988079071</v>
+        <v>22.50000057369471</v>
       </c>
       <c r="J28" t="n">
-        <v>22.50000057369471</v>
-      </c>
-      <c r="K28" t="n">
         <v>859</v>
       </c>
     </row>
@@ -1625,12 +1539,9 @@
         <v>96.09999847412109</v>
       </c>
       <c r="I29" t="n">
-        <v>18.30000042915344</v>
+        <v>18.89999914169312</v>
       </c>
       <c r="J29" t="n">
-        <v>18.89999914169312</v>
-      </c>
-      <c r="K29" t="n">
         <v>106</v>
       </c>
     </row>
@@ -1666,12 +1577,9 @@
         <v>23.39999961853027</v>
       </c>
       <c r="I30" t="n">
-        <v>0.699999988079071</v>
+        <v>10.89999961853027</v>
       </c>
       <c r="J30" t="n">
-        <v>10.89999961853027</v>
-      </c>
-      <c r="K30" t="n">
         <v>79</v>
       </c>
     </row>
@@ -1707,12 +1615,9 @@
         <v>71.09999924898148</v>
       </c>
       <c r="I31" t="n">
-        <v>3.300000071525574</v>
+        <v>29.20000039041042</v>
       </c>
       <c r="J31" t="n">
-        <v>29.20000039041042</v>
-      </c>
-      <c r="K31" t="n">
         <v>516</v>
       </c>
     </row>
@@ -1748,12 +1653,9 @@
         <v>23.10000038146973</v>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>8.599999904632568</v>
       </c>
       <c r="J32" t="n">
-        <v>8.599999904632568</v>
-      </c>
-      <c r="K32" t="n">
         <v>352</v>
       </c>
     </row>
@@ -1789,12 +1691,9 @@
         <v>48.10000076889992</v>
       </c>
       <c r="I33" t="n">
-        <v>4.400000095367432</v>
+        <v>62.49999904632568</v>
       </c>
       <c r="J33" t="n">
-        <v>62.49999904632568</v>
-      </c>
-      <c r="K33" t="n">
         <v>427</v>
       </c>
     </row>
@@ -1830,12 +1729,9 @@
         <v>104.0000038146973</v>
       </c>
       <c r="I34" t="n">
-        <v>4.500000193715096</v>
+        <v>83.5</v>
       </c>
       <c r="J34" t="n">
-        <v>83.5</v>
-      </c>
-      <c r="K34" t="n">
         <v>1251</v>
       </c>
     </row>
@@ -1871,12 +1767,9 @@
         <v>74.30000162124634</v>
       </c>
       <c r="I35" t="n">
-        <v>7.699999809265137</v>
+        <v>15.5999998152256</v>
       </c>
       <c r="J35" t="n">
-        <v>15.5999998152256</v>
-      </c>
-      <c r="K35" t="n">
         <v>316</v>
       </c>
     </row>
@@ -1912,12 +1805,9 @@
         <v>58.89999961853027</v>
       </c>
       <c r="I36" t="n">
-        <v>4.900000095367432</v>
+        <v>14.70000028610229</v>
       </c>
       <c r="J36" t="n">
-        <v>14.70000028610229</v>
-      </c>
-      <c r="K36" t="n">
         <v>283</v>
       </c>
     </row>
@@ -1953,12 +1843,9 @@
         <v>145.4000024795532</v>
       </c>
       <c r="I37" t="n">
-        <v>16.39999973773956</v>
+        <v>34.99999926239252</v>
       </c>
       <c r="J37" t="n">
-        <v>34.99999926239252</v>
-      </c>
-      <c r="K37" t="n">
         <v>143</v>
       </c>
     </row>
@@ -1994,12 +1881,9 @@
         <v>68.89999914169312</v>
       </c>
       <c r="I38" t="n">
-        <v>6.599999904632568</v>
+        <v>27.30000038444996</v>
       </c>
       <c r="J38" t="n">
-        <v>27.30000038444996</v>
-      </c>
-      <c r="K38" t="n">
         <v>888</v>
       </c>
     </row>
@@ -2035,12 +1919,9 @@
         <v>87.40000152587891</v>
       </c>
       <c r="I39" t="n">
-        <v>7.200000047683716</v>
+        <v>3.300000049173832</v>
       </c>
       <c r="J39" t="n">
-        <v>3.300000049173832</v>
-      </c>
-      <c r="K39" t="n">
         <v>263</v>
       </c>
     </row>
@@ -2076,12 +1957,9 @@
         <v>44.29999846220016</v>
       </c>
       <c r="I40" t="n">
-        <v>5.099999964237213</v>
+        <v>39.59999942779541</v>
       </c>
       <c r="J40" t="n">
-        <v>39.59999942779541</v>
-      </c>
-      <c r="K40" t="n">
         <v>576</v>
       </c>
     </row>
@@ -2117,12 +1995,9 @@
         <v>262.0000076293945</v>
       </c>
       <c r="I41" t="n">
-        <v>35.09999942779541</v>
+        <v>115.0000038146973</v>
       </c>
       <c r="J41" t="n">
-        <v>115.0000038146973</v>
-      </c>
-      <c r="K41" t="n">
         <v>2194</v>
       </c>
     </row>
@@ -2158,12 +2033,9 @@
         <v>88.09999847412109</v>
       </c>
       <c r="I42" t="n">
-        <v>12.59999966621399</v>
+        <v>40.99999904632568</v>
       </c>
       <c r="J42" t="n">
-        <v>40.99999904632568</v>
-      </c>
-      <c r="K42" t="n">
         <v>630</v>
       </c>
     </row>
@@ -2199,12 +2071,9 @@
         <v>45.8999981880188</v>
       </c>
       <c r="I43" t="n">
-        <v>5.50000011920929</v>
+        <v>24.99999924004078</v>
       </c>
       <c r="J43" t="n">
-        <v>24.99999924004078</v>
-      </c>
-      <c r="K43" t="n">
         <v>411</v>
       </c>
     </row>
@@ -2240,12 +2109,9 @@
         <v>53</v>
       </c>
       <c r="I44" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J44" t="n">
-        <v>8</v>
-      </c>
-      <c r="K44" t="n">
         <v>85.69999980926514</v>
       </c>
     </row>
@@ -2281,12 +2147,9 @@
         <v>31</v>
       </c>
       <c r="I45" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="J45" t="n">
-        <v>22</v>
-      </c>
-      <c r="K45" t="n">
         <v>1119.200012207031</v>
       </c>
     </row>
@@ -2322,12 +2185,9 @@
         <v>87</v>
       </c>
       <c r="I46" t="n">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="J46" t="n">
-        <v>47</v>
-      </c>
-      <c r="K46" t="n">
         <v>1834.300048828125</v>
       </c>
     </row>
@@ -2362,12 +2222,9 @@
         <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="J47" t="n">
-        <v>12</v>
-      </c>
-      <c r="K47" t="n">
         <v>534.0999755859375</v>
       </c>
     </row>
@@ -2402,12 +2259,9 @@
         <v>72</v>
       </c>
       <c r="I48" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J48" t="n">
-        <v>15</v>
-      </c>
-      <c r="K48" t="n">
         <v>993.5</v>
       </c>
     </row>
@@ -2443,12 +2297,9 @@
         <v>108</v>
       </c>
       <c r="I49" t="n">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="J49" t="n">
-        <v>48</v>
-      </c>
-      <c r="K49" t="n">
         <v>949.4999878406525</v>
       </c>
     </row>
@@ -2484,12 +2335,9 @@
         <v>54</v>
       </c>
       <c r="I50" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J50" t="n">
-        <v>15</v>
-      </c>
-      <c r="K50" t="n">
         <v>424.8000059127808</v>
       </c>
     </row>
@@ -2525,12 +2373,9 @@
         <v>13</v>
       </c>
       <c r="I51" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J51" t="n">
-        <v>7</v>
-      </c>
-      <c r="K51" t="n">
         <v>37</v>
       </c>
     </row>
@@ -2566,12 +2411,9 @@
         <v>74</v>
       </c>
       <c r="I52" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="J52" t="n">
-        <v>34</v>
-      </c>
-      <c r="K52" t="n">
         <v>923.5000228881836</v>
       </c>
     </row>
@@ -2607,12 +2449,9 @@
         <v>65</v>
       </c>
       <c r="I53" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J53" t="n">
-        <v>7</v>
-      </c>
-      <c r="K53" t="n">
         <v>341.3999938964844</v>
       </c>
     </row>
@@ -2648,12 +2487,9 @@
         <v>31</v>
       </c>
       <c r="I54" t="n">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="J54" t="n">
-        <v>33</v>
-      </c>
-      <c r="K54" t="n">
         <v>748.0000228881836</v>
       </c>
     </row>
@@ -2689,12 +2525,9 @@
         <v>50</v>
       </c>
       <c r="I55" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J55" t="n">
-        <v>8</v>
-      </c>
-      <c r="K55" t="n">
         <v>63.20000153779984</v>
       </c>
     </row>
@@ -2730,12 +2563,9 @@
         <v>56</v>
       </c>
       <c r="I56" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J56" t="n">
-        <v>6</v>
-      </c>
-      <c r="K56" t="n">
         <v>582.5000028610229</v>
       </c>
     </row>
@@ -2771,12 +2601,9 @@
         <v>63</v>
       </c>
       <c r="I57" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="J57" t="n">
-        <v>29</v>
-      </c>
-      <c r="K57" t="n">
         <v>1107.900012016296</v>
       </c>
     </row>
@@ -2812,12 +2639,9 @@
         <v>78</v>
       </c>
       <c r="I58" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J58" t="n">
-        <v>7</v>
-      </c>
-      <c r="K58" t="n">
         <v>361.4999878406525</v>
       </c>
     </row>
@@ -2853,12 +2677,9 @@
         <v>36</v>
       </c>
       <c r="I59" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J59" t="n">
-        <v>2</v>
-      </c>
-      <c r="K59" t="n">
         <v>535.7999877929688</v>
       </c>
     </row>
@@ -2894,12 +2715,9 @@
         <v>89</v>
       </c>
       <c r="I60" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="J60" t="n">
-        <v>27</v>
-      </c>
-      <c r="K60" t="n">
         <v>734.7999877929688</v>
       </c>
     </row>
@@ -2935,12 +2753,9 @@
         <v>80</v>
       </c>
       <c r="I61" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="J61" t="n">
-        <v>18</v>
-      </c>
-      <c r="K61" t="n">
         <v>206.0000030994415</v>
       </c>
     </row>
@@ -2976,12 +2791,9 @@
         <v>111</v>
       </c>
       <c r="I62" t="n">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="J62" t="n">
-        <v>59</v>
-      </c>
-      <c r="K62" t="n">
         <v>1660.700012207031</v>
       </c>
     </row>
@@ -3017,12 +2829,9 @@
         <v>84</v>
       </c>
       <c r="I63" t="n">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="J63" t="n">
-        <v>46</v>
-      </c>
-      <c r="K63" t="n">
         <v>1823.5</v>
       </c>
     </row>
@@ -3058,12 +2867,9 @@
         <v>74</v>
       </c>
       <c r="I64" t="n">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="J64" t="n">
-        <v>35</v>
-      </c>
-      <c r="K64" t="n">
         <v>797.900012254715</v>
       </c>
     </row>
@@ -3098,12 +2904,9 @@
         <v>40</v>
       </c>
       <c r="I65" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J65" t="n">
-        <v>3</v>
-      </c>
-      <c r="K65" t="n">
         <v>1021</v>
       </c>
     </row>
@@ -3138,12 +2941,9 @@
         <v>57</v>
       </c>
       <c r="I66" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J66" t="n">
-        <v>11</v>
-      </c>
-      <c r="K66" t="n">
         <v>816</v>
       </c>
     </row>
@@ -3178,12 +2978,9 @@
         <v>96</v>
       </c>
       <c r="I67" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="J67" t="n">
-        <v>49</v>
-      </c>
-      <c r="K67" t="n">
         <v>1107</v>
       </c>
     </row>
@@ -3217,12 +3014,9 @@
         <v>44</v>
       </c>
       <c r="I68" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="J68" t="n">
-        <v>16</v>
-      </c>
-      <c r="K68" t="n">
         <v>1046</v>
       </c>
     </row>
@@ -3256,12 +3050,9 @@
         <v>66</v>
       </c>
       <c r="I69" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J69" t="n">
-        <v>14</v>
-      </c>
-      <c r="K69" t="n">
         <v>1333</v>
       </c>
     </row>
@@ -3296,12 +3087,9 @@
         <v>49</v>
       </c>
       <c r="I70" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J70" t="n">
-        <v>14</v>
-      </c>
-      <c r="K70" t="n">
         <v>861</v>
       </c>
     </row>
@@ -3336,12 +3124,9 @@
         <v>78</v>
       </c>
       <c r="I71" t="n">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="J71" t="n">
-        <v>51</v>
-      </c>
-      <c r="K71" t="n">
         <v>1416</v>
       </c>
     </row>
@@ -3376,12 +3161,9 @@
         <v>20</v>
       </c>
       <c r="I72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K72" t="n">
         <v>4</v>
       </c>
     </row>
@@ -3416,12 +3198,9 @@
         <v>153</v>
       </c>
       <c r="I73" t="n">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="J73" t="n">
-        <v>49</v>
-      </c>
-      <c r="K73" t="n">
         <v>2438</v>
       </c>
     </row>
@@ -3456,12 +3235,9 @@
         <v>66</v>
       </c>
       <c r="I74" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="J74" t="n">
-        <v>30</v>
-      </c>
-      <c r="K74" t="n">
         <v>1079</v>
       </c>
     </row>
@@ -3496,12 +3272,9 @@
         <v>54</v>
       </c>
       <c r="I75" t="n">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="J75" t="n">
-        <v>35</v>
-      </c>
-      <c r="K75" t="n">
         <v>1279</v>
       </c>
     </row>
@@ -3536,12 +3309,9 @@
         <v>114</v>
       </c>
       <c r="I76" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J76" t="n">
-        <v>12</v>
-      </c>
-      <c r="K76" t="n">
         <v>1496</v>
       </c>
     </row>
@@ -3579,9 +3349,6 @@
         <v>17</v>
       </c>
       <c r="J77" t="n">
-        <v>17</v>
-      </c>
-      <c r="K77" t="n">
         <v>2098</v>
       </c>
     </row>
@@ -3616,12 +3383,9 @@
         <v>28</v>
       </c>
       <c r="I78" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J78" t="n">
-        <v>11</v>
-      </c>
-      <c r="K78" t="n">
         <v>1414</v>
       </c>
     </row>
@@ -3656,12 +3420,9 @@
         <v>90</v>
       </c>
       <c r="I79" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J79" t="n">
-        <v>16</v>
-      </c>
-      <c r="K79" t="n">
         <v>1232</v>
       </c>
     </row>
@@ -3696,12 +3457,9 @@
         <v>55</v>
       </c>
       <c r="I80" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J80" t="n">
-        <v>14</v>
-      </c>
-      <c r="K80" t="n">
         <v>1739</v>
       </c>
     </row>
@@ -3736,12 +3494,9 @@
         <v>100</v>
       </c>
       <c r="I81" t="n">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="J81" t="n">
-        <v>33</v>
-      </c>
-      <c r="K81" t="n">
         <v>1239</v>
       </c>
     </row>
@@ -3776,12 +3531,9 @@
         <v>46</v>
       </c>
       <c r="I82" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J82" t="n">
-        <v>17</v>
-      </c>
-      <c r="K82" t="n">
         <v>1248</v>
       </c>
     </row>
@@ -3816,12 +3568,9 @@
         <v>156</v>
       </c>
       <c r="I83" t="n">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="J83" t="n">
-        <v>62</v>
-      </c>
-      <c r="K83" t="n">
         <v>2599</v>
       </c>
     </row>
@@ -3856,12 +3605,9 @@
         <v>105</v>
       </c>
       <c r="I84" t="n">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="J84" t="n">
-        <v>43</v>
-      </c>
-      <c r="K84" t="n">
         <v>2164</v>
       </c>
     </row>
@@ -3896,12 +3642,9 @@
         <v>46</v>
       </c>
       <c r="I85" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J85" t="n">
-        <v>15</v>
-      </c>
-      <c r="K85" t="n">
         <v>963</v>
       </c>
     </row>
@@ -3936,12 +3679,9 @@
         <v>77.94999694824219</v>
       </c>
       <c r="I86" t="n">
-        <v>9.020000457763672</v>
+        <v>31.77000045776367</v>
       </c>
       <c r="J86" t="n">
-        <v>31.77000045776367</v>
-      </c>
-      <c r="K86" t="n">
         <v>907.2000122070312</v>
       </c>
     </row>
@@ -3976,12 +3716,9 @@
         <v>75.75015258789062</v>
       </c>
       <c r="I87" t="n">
-        <v>5.816500186920166</v>
+        <v>24.86395072937012</v>
       </c>
       <c r="J87" t="n">
-        <v>24.86395072937012</v>
-      </c>
-      <c r="K87" t="n">
         <v>680.5</v>
       </c>
     </row>
@@ -4016,12 +3753,9 @@
         <v>71.90000152587891</v>
       </c>
       <c r="I88" t="n">
-        <v>5.355000019073486</v>
+        <v>52.33499908447266</v>
       </c>
       <c r="J88" t="n">
-        <v>52.33499908447266</v>
-      </c>
-      <c r="K88" t="n">
         <v>1036.579956054688</v>
       </c>
     </row>
@@ -4055,12 +3789,9 @@
         <v>84.08000183105469</v>
       </c>
       <c r="I89" t="n">
-        <v>3.960000038146973</v>
+        <v>25.93000030517578</v>
       </c>
       <c r="J89" t="n">
-        <v>25.93000030517578</v>
-      </c>
-      <c r="K89" t="n">
         <v>1165.487060546875</v>
       </c>
     </row>
@@ -4094,12 +3825,9 @@
         <v>64.50015258789062</v>
       </c>
       <c r="I90" t="n">
-        <v>5.346499919891357</v>
+        <v>34.97394943237305</v>
       </c>
       <c r="J90" t="n">
-        <v>34.97394943237305</v>
-      </c>
-      <c r="K90" t="n">
         <v>684.10498046875</v>
       </c>
     </row>
@@ -4134,12 +3862,9 @@
         <v>56.59000015258789</v>
       </c>
       <c r="I91" t="n">
-        <v>9.409999847412109</v>
+        <v>34.90000152587891</v>
       </c>
       <c r="J91" t="n">
-        <v>34.90000152587891</v>
-      </c>
-      <c r="K91" t="n">
         <v>551.72998046875</v>
       </c>
     </row>
@@ -4174,12 +3899,9 @@
         <v>70.91000366210938</v>
       </c>
       <c r="I92" t="n">
-        <v>10.15499973297119</v>
+        <v>33.02999877929688</v>
       </c>
       <c r="J92" t="n">
-        <v>33.02999877929688</v>
-      </c>
-      <c r="K92" t="n">
         <v>681.47998046875</v>
       </c>
     </row>
@@ -4214,12 +3936,9 @@
         <v>12.35000038146973</v>
       </c>
       <c r="I93" t="n">
-        <v>0</v>
+        <v>2.507999897003174</v>
       </c>
       <c r="J93" t="n">
-        <v>2.507999897003174</v>
-      </c>
-      <c r="K93" t="n">
         <v>81.58000183105469</v>
       </c>
     </row>
@@ -4254,12 +3973,9 @@
         <v>97.02999877929688</v>
       </c>
       <c r="I94" t="n">
-        <v>5.309999942779541</v>
+        <v>43.18000030517578</v>
       </c>
       <c r="J94" t="n">
-        <v>43.18000030517578</v>
-      </c>
-      <c r="K94" t="n">
         <v>741.5700073242188</v>
       </c>
     </row>
@@ -4294,12 +4010,9 @@
         <v>30.61499977111816</v>
       </c>
       <c r="I95" t="n">
-        <v>1.409999966621399</v>
+        <v>23.70499992370605</v>
       </c>
       <c r="J95" t="n">
-        <v>23.70499992370605</v>
-      </c>
-      <c r="K95" t="n">
         <v>472.010009765625</v>
       </c>
     </row>
@@ -4334,12 +4047,9 @@
         <v>77.23000335693359</v>
       </c>
       <c r="I96" t="n">
-        <v>4.110000133514404</v>
+        <v>51.02999877929688</v>
       </c>
       <c r="J96" t="n">
-        <v>51.02999877929688</v>
-      </c>
-      <c r="K96" t="n">
         <v>793.0700073242188</v>
       </c>
     </row>
@@ -4374,12 +4084,9 @@
         <v>89.84500122070312</v>
       </c>
       <c r="I97" t="n">
-        <v>5.5</v>
+        <v>32.52500152587891</v>
       </c>
       <c r="J97" t="n">
-        <v>32.52500152587891</v>
-      </c>
-      <c r="K97" t="n">
         <v>541.8300170898438</v>
       </c>
     </row>
@@ -4414,12 +4121,9 @@
         <v>104.1989974975586</v>
       </c>
       <c r="I98" t="n">
-        <v>8.875</v>
+        <v>11.20199966430664</v>
       </c>
       <c r="J98" t="n">
-        <v>11.20199966430664</v>
-      </c>
-      <c r="K98" t="n">
         <v>912.02001953125</v>
       </c>
     </row>
@@ -4454,12 +4158,9 @@
         <v>75.55000305175781</v>
       </c>
       <c r="I99" t="n">
-        <v>6.880000114440918</v>
-      </c>
-      <c r="J99" t="n">
         <v>26.68000030517578</v>
       </c>
-      <c r="K99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -4492,12 +4193,9 @@
         <v>75</v>
       </c>
       <c r="I100" t="n">
-        <v>10.13500022888184</v>
+        <v>25.67499923706055</v>
       </c>
       <c r="J100" t="n">
-        <v>25.67499923706055</v>
-      </c>
-      <c r="K100" t="n">
         <v>532.1300048828125</v>
       </c>
     </row>
@@ -4532,12 +4230,9 @@
         <v>72.24015045166016</v>
       </c>
       <c r="I101" t="n">
-        <v>5.596499919891357</v>
+        <v>28.4239501953125</v>
       </c>
       <c r="J101" t="n">
-        <v>28.4239501953125</v>
-      </c>
-      <c r="K101" t="n">
         <v>708.510009765625</v>
       </c>
     </row>
@@ -4572,12 +4267,9 @@
         <v>88.87200164794922</v>
       </c>
       <c r="I102" t="n">
-        <v>6.902500152587891</v>
+        <v>28.70549964904785</v>
       </c>
       <c r="J102" t="n">
-        <v>28.70549964904785</v>
-      </c>
-      <c r="K102" t="n">
         <v>799.9650268554688</v>
       </c>
     </row>
@@ -4612,12 +4304,9 @@
         <v>59.06499862670898</v>
       </c>
       <c r="I103" t="n">
-        <v>10.65999984741211</v>
+        <v>32.00500106811523</v>
       </c>
       <c r="J103" t="n">
-        <v>32.00500106811523</v>
-      </c>
-      <c r="K103" t="n">
         <v>559.9299926757812</v>
       </c>
     </row>
@@ -4652,12 +4341,9 @@
         <v>95.09833526611328</v>
       </c>
       <c r="I104" t="n">
-        <v>5.199999809265137</v>
+        <v>36.95999908447266</v>
       </c>
       <c r="J104" t="n">
-        <v>36.95999908447266</v>
-      </c>
-      <c r="K104" t="n">
         <v>687.3800048828125</v>
       </c>
     </row>
@@ -4692,12 +4378,9 @@
         <v>69.05000305175781</v>
       </c>
       <c r="I105" t="n">
-        <v>8.170000076293945</v>
+        <v>31.6299991607666</v>
       </c>
       <c r="J105" t="n">
-        <v>31.6299991607666</v>
-      </c>
-      <c r="K105" t="n">
         <v>1021.77001953125</v>
       </c>
     </row>
@@ -4732,12 +4415,9 @@
         <v>52.52000045776367</v>
       </c>
       <c r="I106" t="n">
-        <v>7.795000076293945</v>
+        <v>42.20500183105469</v>
       </c>
       <c r="J106" t="n">
-        <v>42.20500183105469</v>
-      </c>
-      <c r="K106" t="n">
         <v>491.4800109863281</v>
       </c>
     </row>

</xml_diff>